<commit_message>
220708 exo brain 10,000 sents
</commit_message>
<xml_diff>
--- a/오류분석/Tokenizing_오류.xlsx
+++ b/오류분석/Tokenizing_오류.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATAGI\Desktop\Git\NER-Model\오류분석\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE75C0EC-910B-4B73-BC6A-EBA442DE6946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC73B83-4C7A-4FE6-86FA-E65C30C0C634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20790" yWindow="945" windowWidth="17820" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>개체명 분석 말뭉치 Tokenizing 오류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,13 +51,204 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>개혁 성향의 한 의원은 “‘중도강화론’을 주창한 이 대통령이 유럽 순방을 마치고 돌아오는 7월 중순께 한승수 국무총리, 정정길 대통령 실장, 안병만 교육부 장관 등을 교체하기로 한 것으로 알고 있다”고 말했다.</t>
-  </si>
-  <si>
     <t>오는 7월 중순께</t>
   </si>
   <si>
     <t>돌아오##는 7##월 중순께</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>조지 W 부시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 전 대통령의 회고록 ‘결정의 순간’에도 대북 영향력 행사를 꺼리는 장쩌민 국가주석에게 “북핵 개발을 외교적으로 풀지 못하면 대북 군사공격을 고려할 수밖에 없다”고 압박하는 대목이 나온다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">독일 슈피겔은 \"21세기 전장에선 전투기보다 값이 싸고 위험도가 낮은 CIA의 무인폭격기에 대한 의존도가 나날이 높아지고 있다. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>오바마</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 취임 후 2년 동안 발사된 무인폭격기 미사일은 조지 W 부시 전 대통령의 임기 8년 동안 발사된 무인폭격기 미사일 수를 넘어선 상태\"라고 전했다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>개혁 성향의 한 의원은 “‘중도강화론’을 주창한 이 대통령이 유럽 순방을 마치고 돌아</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>오는 7월 중순께</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 한승수 국무총리, 정정길 대통령 실장, 안병만 교육부 장관 등을 교체하기로 한 것으로 알고 있다”고 말했다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조지 W 부시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오바마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오바마
+(태깅 안됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조지 W 부시
+(태깅 안됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">북한의 3차 핵실험 이후 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>박근혜 대통령</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 당선인의 대북정책 기조인 ‘한반도 신뢰 프로세스’가 흔들릴 조짐을 보이면서, 북핵 문제와 대북정책 연계 여부가 ‘박근혜표 대북정책’의 가늠자로 떠올랐다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인물 이름/직업 명칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">북한의 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>핵</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">과 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>미사일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 공격 가능성에 대해 미국의 핵우산과 재래식 무기, 미사일방어 등 모든 군사능력을 동원해 사전에 억제하겠다는 내용이다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무기 명칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핵과
+미사일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -65,7 +256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +273,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -137,19 +345,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,29 +654,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:G8"/>
+  <dimension ref="B3:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.625" customWidth="1"/>
     <col min="3" max="3" width="48.625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -461,31 +684,87 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="66" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="2" t="s">
+    </row>
+    <row r="9" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="B11" s="8">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="8">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>